<commit_message>
added major changes in code
</commit_message>
<xml_diff>
--- a/excel_config.xlsx
+++ b/excel_config.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajit.Yadav01\Desktop\link-automator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068CBAA8-EE59-46EB-9CE4-0FBEDA949069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -32,6 +26,18 @@
   </si>
   <si>
     <t>Are you…?</t>
+  </si>
+  <si>
+    <t>What is your marital status</t>
+  </si>
+  <si>
+    <t>How many children under the age of 18 are living in your household? Please reference only the children for which you are the parent or legal guardian. (If there are no children under 18 in your household, please type 0)</t>
+  </si>
+  <si>
+    <t>[1,2]</t>
+  </si>
+  <si>
+    <t>somehting</t>
   </si>
   <si>
     <t>Please insert your zipcode:</t>
@@ -40,14 +46,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -83,31 +96,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -118,10 +135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -159,71 +176,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -251,7 +268,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -274,11 +291,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -287,13 +304,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -303,7 +320,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -312,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -321,7 +338,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -329,10 +346,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -397,23 +414,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="76.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="57.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,27 +436,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
         <v>71601</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed js function and added selenium support
</commit_message>
<xml_diff>
--- a/excel_config.xlsx
+++ b/excel_config.xlsx
@@ -46,7 +46,7 @@
     <t>Please insert your zipcode:</t>
   </si>
   <si>
-    <t>How many children under the age of 18 are living in your household? Please reference only the children for which you are the parent or legal guardian. (If there are no children under 18 in your household, please type 0)</t>
+    <t/>
   </si>
   <si>
     <t>Are you of Hispanic, Latino or Spanish origin?
@@ -101,13 +101,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -423,8 +426,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="76.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="57.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="76.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="57.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -492,12 +495,10 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="58.5">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
intial 1.0 beta need to brush up functions Happy weekends :)
</commit_message>
<xml_diff>
--- a/excel_config.xlsx
+++ b/excel_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">text </t>
   </si>
   <si>
-    <t>[_1,_2]</t>
+    <t>[1,2]</t>
   </si>
   <si>
     <t>What is your current employment status?</t>
@@ -46,10 +46,20 @@
     <t>Please insert your zipcode:</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Are you of Hispanic, Latino or Spanish origin?
+    <t>Please tell us how interested you are in the NHL.</t>
+  </si>
+  <si>
+    <t>The next question will be about race and ethnicity. A “Prefer not to answer” option is available for you to select, at your discretion. Collecting such information enables us to provide a more refined research analysis.
+Participation is always voluntary, and your responses are used for research purposes only, combined with the answers from all other participants. We will provide our client only anonymous, aggregated results. The data will be held for no longer than 12 months.
+Do you accept the collection of race and ethnicity related data?
+Select only one</t>
+  </si>
+  <si>
+    <t>Which of the following subscription streaming services do you subscribe to?</t>
+  </si>
+  <si>
+    <t>This is a topic of a sensitive nature. Answering is voluntary, however, collecting such information enables us to provide a more refined research analysis.
+Are you of Hispanic, Latino or Spanish origin?
 If you don’t agree to provide us such information, a “Prefer not to answer” option is available for you to select, at your discretion.
 For any survey research purposes, your responses are combined with the answers from all other participants. We will provide our client only anonymous results, unless you separately consent otherwise. The data will be held by us for the research purposes no longer than 12 months.</t>
   </si>
@@ -59,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +80,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -101,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -109,8 +125,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -420,14 +439,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="76.57642857142856" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="57.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="76.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="57.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -495,16 +514,34 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="58.5">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="87">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="60">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
thak gaya hun abhi baad mein karta hu :):
</commit_message>
<xml_diff>
--- a/excel_config.xlsx
+++ b/excel_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>What is your current employment status?</t>
+  </si>
+  <si>
+    <t>How many children under the age of 18 are living in your household? Please reference only the children for which you are the parent or legal guardian. (If there are no children under 18 in your household, please type 0)</t>
   </si>
   <si>
     <t>Please insert your zipcode:</t>
@@ -56,6 +59,12 @@
   </si>
   <si>
     <t>Which of the following subscription streaming services do you subscribe to?</t>
+  </si>
+  <si>
+    <t>Please tell us how often you typically watch the NHL streaming on Hulu on your tablet, smartphone, smart TV or streaming device (Roku, Apple TV, Amazon TV Fire stick, etc.).</t>
+  </si>
+  <si>
+    <t>rrrrrrrrrr</t>
   </si>
   <si>
     <t>This is a topic of a sensitive nature. Answering is voluntary, however, collecting such information enables us to provide a more refined research analysis.
@@ -125,10 +134,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -439,7 +448,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -505,12 +514,12 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
-        <v>71601</v>
+      <c r="B8" s="3">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -518,18 +527,18 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="87">
+        <v>71601</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="87">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -537,11 +546,27 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="60">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="60">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
work on multi question on one screen
</commit_message>
<xml_diff>
--- a/excel_config.xlsx
+++ b/excel_config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Question</t>
   </si>
@@ -28,7 +28,8 @@
     <t>Are you…?</t>
   </si>
   <si>
-    <t>What is your marital status</t>
+    <t>What is your marital status?
+Select only one</t>
   </si>
   <si>
     <t>somehting</t>
@@ -44,6 +45,9 @@
   </si>
   <si>
     <t>How many children under the age of 18 are living in your household? Please reference only the children for which you are the parent or legal guardian. (If there are no children under 18 in your household, please type 0)</t>
+  </si>
+  <si>
+    <t>'0'</t>
   </si>
   <si>
     <t>Please insert your zipcode:</t>
@@ -129,19 +133,19 @@
   <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -482,12 +486,12 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="32.25">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -514,17 +518,17 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>71601</v>
@@ -532,39 +536,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="87">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="135.75">
       <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="3">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="32.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="60">
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="148.5">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>

</xml_diff>